<commit_message>
45/15 + wall + python comments
</commit_message>
<xml_diff>
--- a/datalibrary.xlsx
+++ b/datalibrary.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="948">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="951">
   <si>
     <t>Test File</t>
   </si>
@@ -2858,6 +2858,15 @@
   </si>
   <si>
     <t>test_170625b.csv</t>
+  </si>
+  <si>
+    <t>www_170626a.txt</t>
+  </si>
+  <si>
+    <t>www_170626a.csv</t>
+  </si>
+  <si>
+    <t>www</t>
   </si>
 </sst>
 </file>
@@ -4145,7 +4154,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I452"/>
+  <dimension ref="A1:I453"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A403" workbookViewId="0" zoomScale="110" zoomScaleNormal="110">
       <selection activeCell="A417" sqref="A417:XFD417"/>
@@ -17266,6 +17275,35 @@
         <v>0</v>
       </c>
     </row>
+    <row r="453" spans="1:9">
+      <c r="A453" t="s">
+        <v>948</v>
+      </c>
+      <c r="B453" t="s">
+        <v>949</v>
+      </c>
+      <c r="C453" t="s">
+        <v>950</v>
+      </c>
+      <c r="D453" t="n">
+        <v>170626</v>
+      </c>
+      <c r="E453" t="s">
+        <v>12</v>
+      </c>
+      <c r="F453" t="n">
+        <v>222</v>
+      </c>
+      <c r="G453" t="n">
+        <v>6</v>
+      </c>
+      <c r="H453" t="n">
+        <v>3</v>
+      </c>
+      <c r="I453" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait"/>

</xml_diff>

<commit_message>
plot correct number of boxes
</commit_message>
<xml_diff>
--- a/datalibrary.xlsx
+++ b/datalibrary.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="951">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="965">
   <si>
     <t>Test File</t>
   </si>
@@ -2867,6 +2867,48 @@
   </si>
   <si>
     <t>www</t>
+  </si>
+  <si>
+    <t>www_170626b.txt</t>
+  </si>
+  <si>
+    <t>www_170626b.csv</t>
+  </si>
+  <si>
+    <t>wwww_170626a.txt</t>
+  </si>
+  <si>
+    <t>wwww_170626a.csv</t>
+  </si>
+  <si>
+    <t>wwww</t>
+  </si>
+  <si>
+    <t>pietro_170626a.txt</t>
+  </si>
+  <si>
+    <t>pietro_170626a.csv</t>
+  </si>
+  <si>
+    <t>pietro</t>
+  </si>
+  <si>
+    <t>io_170626a.txt</t>
+  </si>
+  <si>
+    <t>io_170626a.csv</t>
+  </si>
+  <si>
+    <t>io</t>
+  </si>
+  <si>
+    <t>weila_170626a.txt</t>
+  </si>
+  <si>
+    <t>weila_170626a.csv</t>
+  </si>
+  <si>
+    <t>weila</t>
   </si>
 </sst>
 </file>
@@ -4154,7 +4196,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I453"/>
+  <dimension ref="A1:I458"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A403" workbookViewId="0" zoomScale="110" zoomScaleNormal="110">
       <selection activeCell="A417" sqref="A417:XFD417"/>
@@ -17304,6 +17346,151 @@
         <v>0</v>
       </c>
     </row>
+    <row r="454" spans="1:9">
+      <c r="A454" t="s">
+        <v>951</v>
+      </c>
+      <c r="B454" t="s">
+        <v>952</v>
+      </c>
+      <c r="C454" t="s">
+        <v>950</v>
+      </c>
+      <c r="D454" t="n">
+        <v>170626</v>
+      </c>
+      <c r="E454" t="s">
+        <v>108</v>
+      </c>
+      <c r="F454" t="n">
+        <v>12222</v>
+      </c>
+      <c r="G454" t="n">
+        <v>6</v>
+      </c>
+      <c r="H454" t="n">
+        <v>3</v>
+      </c>
+      <c r="I454" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="455" spans="1:9">
+      <c r="A455" t="s">
+        <v>953</v>
+      </c>
+      <c r="B455" t="s">
+        <v>954</v>
+      </c>
+      <c r="C455" t="s">
+        <v>955</v>
+      </c>
+      <c r="D455" t="n">
+        <v>170626</v>
+      </c>
+      <c r="E455" t="s">
+        <v>12</v>
+      </c>
+      <c r="F455" t="n">
+        <v>122</v>
+      </c>
+      <c r="G455" t="n">
+        <v>6</v>
+      </c>
+      <c r="H455" t="n">
+        <v>3</v>
+      </c>
+      <c r="I455" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="456" spans="1:9">
+      <c r="A456" t="s">
+        <v>956</v>
+      </c>
+      <c r="B456" t="s">
+        <v>957</v>
+      </c>
+      <c r="C456" t="s">
+        <v>958</v>
+      </c>
+      <c r="D456" t="n">
+        <v>170626</v>
+      </c>
+      <c r="E456" t="s">
+        <v>12</v>
+      </c>
+      <c r="F456" t="n">
+        <v>67</v>
+      </c>
+      <c r="G456" t="n">
+        <v>6</v>
+      </c>
+      <c r="H456" t="n">
+        <v>3</v>
+      </c>
+      <c r="I456" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="457" spans="1:9">
+      <c r="A457" t="s">
+        <v>959</v>
+      </c>
+      <c r="B457" t="s">
+        <v>960</v>
+      </c>
+      <c r="C457" t="s">
+        <v>961</v>
+      </c>
+      <c r="D457" t="n">
+        <v>170626</v>
+      </c>
+      <c r="E457" t="s">
+        <v>12</v>
+      </c>
+      <c r="F457" t="n">
+        <v>22</v>
+      </c>
+      <c r="G457" t="n">
+        <v>6</v>
+      </c>
+      <c r="H457" t="n">
+        <v>3</v>
+      </c>
+      <c r="I457" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="458" spans="1:9">
+      <c r="A458" t="s">
+        <v>962</v>
+      </c>
+      <c r="B458" t="s">
+        <v>963</v>
+      </c>
+      <c r="C458" t="s">
+        <v>964</v>
+      </c>
+      <c r="D458" t="n">
+        <v>170626</v>
+      </c>
+      <c r="E458" t="s">
+        <v>12</v>
+      </c>
+      <c r="F458" t="n">
+        <v>22</v>
+      </c>
+      <c r="G458" t="n">
+        <v>6</v>
+      </c>
+      <c r="H458" t="n">
+        <v>3</v>
+      </c>
+      <c r="I458" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait"/>

</xml_diff>